<commit_message>
Overview of tags and detections
</commit_message>
<xml_diff>
--- a/Data/Tag detections log_Sept 22-April 23.xlsx
+++ b/Data/Tag detections log_Sept 22-April 23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Palau\Research\Coastal Fisheries\Natalie Tagging\2022 Bohar tagging\Bohar_2022_2023\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE13463-6F2A-46F4-9DB3-94C50064DC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2247AD53-C1EC-4FE1-AD51-18A274766526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="20">
   <si>
     <t>Tag</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Only two days detected</t>
+  </si>
+  <si>
+    <t>Only at Siaes Corner</t>
   </si>
 </sst>
 </file>
@@ -403,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1005,6 +1008,12 @@
       <c r="G25" t="s">
         <v>9</v>
       </c>
+      <c r="H25">
+        <v>25</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
       <c r="J25" t="s">
         <v>16</v>
       </c>
@@ -1031,6 +1040,15 @@
       <c r="G26" t="s">
         <v>9</v>
       </c>
+      <c r="H26">
+        <v>4322</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
@@ -1054,6 +1072,12 @@
       <c r="G27" t="s">
         <v>9</v>
       </c>
+      <c r="H27">
+        <v>963</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
@@ -1069,13 +1093,19 @@
         <v>45031</v>
       </c>
       <c r="E28" s="2">
-        <v>44812</v>
+        <v>44867</v>
       </c>
       <c r="F28" s="2">
-        <v>44813</v>
+        <v>45019</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
+      </c>
+      <c r="H28">
+        <v>3688</v>
+      </c>
+      <c r="I28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1100,6 +1130,12 @@
       <c r="G29" t="s">
         <v>9</v>
       </c>
+      <c r="H29">
+        <v>270</v>
+      </c>
+      <c r="I29" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
@@ -1123,6 +1159,12 @@
       <c r="G30" t="s">
         <v>9</v>
       </c>
+      <c r="H30">
+        <v>24848</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
@@ -1146,6 +1188,12 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
+      <c r="H31">
+        <v>49</v>
+      </c>
+      <c r="I31" t="s">
+        <v>12</v>
+      </c>
       <c r="J31" t="s">
         <v>18</v>
       </c>
@@ -1172,6 +1220,12 @@
       <c r="G32" t="s">
         <v>9</v>
       </c>
+      <c r="H32">
+        <v>2613</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
@@ -1186,6 +1240,21 @@
       <c r="D33" s="1">
         <v>45031</v>
       </c>
+      <c r="E33" s="2">
+        <v>44868</v>
+      </c>
+      <c r="F33" s="2">
+        <v>44990</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>2846</v>
+      </c>
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
@@ -1200,6 +1269,21 @@
       <c r="D34" s="1">
         <v>45031</v>
       </c>
+      <c r="E34" s="2">
+        <v>44868</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44925</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>433</v>
+      </c>
+      <c r="I34" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
@@ -1213,6 +1297,21 @@
       </c>
       <c r="D35" s="1">
         <v>45031</v>
+      </c>
+      <c r="E35" s="2">
+        <v>44869</v>
+      </c>
+      <c r="F35" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>2402</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>